<commit_message>
fix a bug in generate_group
</commit_message>
<xml_diff>
--- a/data/CET6-1500.xlsx
+++ b/data/CET6-1500.xlsx
@@ -9414,7 +9414,7 @@
         <v>1504</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E2" t="b">
         <v>0</v>
@@ -9431,10 +9431,10 @@
         <v>1505</v>
       </c>
       <c r="D3">
+        <v>2</v>
+      </c>
+      <c r="E3" t="b">
         <v>1</v>
-      </c>
-      <c r="E3" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -9448,7 +9448,7 @@
         <v>1506</v>
       </c>
       <c r="D4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E4" t="b">
         <v>0</v>
@@ -9482,10 +9482,10 @@
         <v>1508</v>
       </c>
       <c r="D6">
+        <v>4</v>
+      </c>
+      <c r="E6" t="b">
         <v>1</v>
-      </c>
-      <c r="E6" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -9499,7 +9499,7 @@
         <v>1509</v>
       </c>
       <c r="D7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E7" t="b">
         <v>0</v>
@@ -9533,7 +9533,7 @@
         <v>1511</v>
       </c>
       <c r="D9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E9" t="b">
         <v>0</v>
@@ -9567,7 +9567,7 @@
         <v>1513</v>
       </c>
       <c r="D11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E11" t="b">
         <v>0</v>
@@ -9601,7 +9601,7 @@
         <v>1515</v>
       </c>
       <c r="D13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E13" t="b">
         <v>0</v>
@@ -9669,7 +9669,7 @@
         <v>1519</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E17" t="b">
         <v>0</v>
@@ -9703,7 +9703,7 @@
         <v>1521</v>
       </c>
       <c r="D19">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E19" t="b">
         <v>0</v>
@@ -9924,7 +9924,7 @@
         <v>1534</v>
       </c>
       <c r="D32">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="E32" t="b">
         <v>0</v>
@@ -9941,7 +9941,7 @@
         <v>1535</v>
       </c>
       <c r="D33">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E33" t="b">
         <v>0</v>
@@ -9958,7 +9958,7 @@
         <v>1536</v>
       </c>
       <c r="D34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E34" t="b">
         <v>0</v>
@@ -9975,7 +9975,7 @@
         <v>1537</v>
       </c>
       <c r="D35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E35" t="b">
         <v>0</v>
@@ -10077,7 +10077,7 @@
         <v>1543</v>
       </c>
       <c r="D41">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E41" t="b">
         <v>0</v>
@@ -10094,7 +10094,7 @@
         <v>1544</v>
       </c>
       <c r="D42">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E42" t="b">
         <v>0</v>
@@ -10111,7 +10111,7 @@
         <v>1545</v>
       </c>
       <c r="D43">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E43" t="b">
         <v>0</v>
@@ -10145,7 +10145,7 @@
         <v>1547</v>
       </c>
       <c r="D45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E45" t="b">
         <v>0</v>
@@ -10162,7 +10162,7 @@
         <v>1548</v>
       </c>
       <c r="D46">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E46" t="b">
         <v>0</v>
@@ -10298,7 +10298,7 @@
         <v>1556</v>
       </c>
       <c r="D54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E54" t="b">
         <v>0</v>
@@ -10349,10 +10349,10 @@
         <v>1559</v>
       </c>
       <c r="D57">
+        <v>2</v>
+      </c>
+      <c r="E57" t="b">
         <v>1</v>
-      </c>
-      <c r="E57" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:5">
@@ -10383,7 +10383,7 @@
         <v>1561</v>
       </c>
       <c r="D59">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E59" t="b">
         <v>0</v>
@@ -10417,7 +10417,7 @@
         <v>1563</v>
       </c>
       <c r="D61">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E61" t="b">
         <v>0</v>
@@ -10468,7 +10468,7 @@
         <v>1566</v>
       </c>
       <c r="D64">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E64" t="b">
         <v>0</v>
@@ -10553,7 +10553,7 @@
         <v>1571</v>
       </c>
       <c r="D69">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E69" t="b">
         <v>0</v>
@@ -10825,10 +10825,10 @@
         <v>1587</v>
       </c>
       <c r="D85">
+        <v>2</v>
+      </c>
+      <c r="E85" t="b">
         <v>1</v>
-      </c>
-      <c r="E85" t="b">
-        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -10978,7 +10978,7 @@
         <v>1596</v>
       </c>
       <c r="D94">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E94" t="b">
         <v>0</v>
@@ -10995,7 +10995,7 @@
         <v>1597</v>
       </c>
       <c r="D95">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E95" t="b">
         <v>0</v>
@@ -11131,7 +11131,7 @@
         <v>1605</v>
       </c>
       <c r="D103">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E103" t="b">
         <v>0</v>
@@ -11233,7 +11233,7 @@
         <v>1611</v>
       </c>
       <c r="D109">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E109" t="b">
         <v>0</v>
@@ -11267,7 +11267,7 @@
         <v>1613</v>
       </c>
       <c r="D111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E111" t="b">
         <v>0</v>
@@ -11284,7 +11284,7 @@
         <v>1614</v>
       </c>
       <c r="D112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E112" t="b">
         <v>0</v>
@@ -11301,7 +11301,7 @@
         <v>1615</v>
       </c>
       <c r="D113">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E113" t="b">
         <v>0</v>
@@ -11318,7 +11318,7 @@
         <v>1616</v>
       </c>
       <c r="D114">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E114" t="b">
         <v>0</v>
@@ -11352,7 +11352,7 @@
         <v>1618</v>
       </c>
       <c r="D116">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E116" t="b">
         <v>0</v>
@@ -11386,7 +11386,7 @@
         <v>1620</v>
       </c>
       <c r="D118">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E118" t="b">
         <v>0</v>
@@ -11420,10 +11420,10 @@
         <v>1622</v>
       </c>
       <c r="D120">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E120" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121" spans="1:5">
@@ -11454,7 +11454,7 @@
         <v>1624</v>
       </c>
       <c r="D122">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E122" t="b">
         <v>0</v>
@@ -11471,7 +11471,7 @@
         <v>1625</v>
       </c>
       <c r="D123">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E123" t="b">
         <v>0</v>
@@ -11488,7 +11488,7 @@
         <v>1626</v>
       </c>
       <c r="D124">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E124" t="b">
         <v>0</v>
@@ -11505,7 +11505,7 @@
         <v>1627</v>
       </c>
       <c r="D125">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E125" t="b">
         <v>0</v>
@@ -11522,10 +11522,10 @@
         <v>1628</v>
       </c>
       <c r="D126">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E126" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:5">
@@ -11539,7 +11539,7 @@
         <v>1629</v>
       </c>
       <c r="D127">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E127" t="b">
         <v>0</v>
@@ -11556,7 +11556,7 @@
         <v>1630</v>
       </c>
       <c r="D128">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E128" t="b">
         <v>0</v>
@@ -11573,7 +11573,7 @@
         <v>1631</v>
       </c>
       <c r="D129">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E129" t="b">
         <v>0</v>
@@ -11590,7 +11590,7 @@
         <v>1632</v>
       </c>
       <c r="D130">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E130" t="b">
         <v>0</v>
@@ -11607,7 +11607,7 @@
         <v>1633</v>
       </c>
       <c r="D131">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E131" t="b">
         <v>0</v>
@@ -11624,7 +11624,7 @@
         <v>1634</v>
       </c>
       <c r="D132">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E132" t="b">
         <v>0</v>
@@ -11641,7 +11641,7 @@
         <v>1635</v>
       </c>
       <c r="D133">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E133" t="b">
         <v>0</v>
@@ -11658,7 +11658,7 @@
         <v>1636</v>
       </c>
       <c r="D134">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E134" t="b">
         <v>0</v>
@@ -11675,7 +11675,7 @@
         <v>1637</v>
       </c>
       <c r="D135">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E135" t="b">
         <v>0</v>
@@ -11692,7 +11692,7 @@
         <v>1638</v>
       </c>
       <c r="D136">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E136" t="b">
         <v>0</v>
@@ -11709,7 +11709,7 @@
         <v>1639</v>
       </c>
       <c r="D137">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E137" t="b">
         <v>0</v>
@@ -11726,7 +11726,7 @@
         <v>1640</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E138" t="b">
         <v>0</v>
@@ -11743,10 +11743,10 @@
         <v>1641</v>
       </c>
       <c r="D139">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E139" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -11760,7 +11760,7 @@
         <v>1642</v>
       </c>
       <c r="D140">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E140" t="b">
         <v>0</v>
@@ -11777,10 +11777,10 @@
         <v>1643</v>
       </c>
       <c r="D141">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E141" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -11794,7 +11794,7 @@
         <v>1644</v>
       </c>
       <c r="D142">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E142" t="b">
         <v>0</v>
@@ -11811,10 +11811,10 @@
         <v>1645</v>
       </c>
       <c r="D143">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E143" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -11828,7 +11828,7 @@
         <v>1646</v>
       </c>
       <c r="D144">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E144" t="b">
         <v>0</v>
@@ -11845,7 +11845,7 @@
         <v>1647</v>
       </c>
       <c r="D145">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E145" t="b">
         <v>0</v>
@@ -11862,7 +11862,7 @@
         <v>1648</v>
       </c>
       <c r="D146">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E146" t="b">
         <v>0</v>
@@ -11879,7 +11879,7 @@
         <v>1649</v>
       </c>
       <c r="D147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E147" t="b">
         <v>0</v>
@@ -11913,7 +11913,7 @@
         <v>1651</v>
       </c>
       <c r="D149">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E149" t="b">
         <v>0</v>
@@ -11947,7 +11947,7 @@
         <v>1653</v>
       </c>
       <c r="D151">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E151" t="b">
         <v>0</v>

</xml_diff>